<commit_message>
Add get_tickers function to broker
</commit_message>
<xml_diff>
--- a/settings/tickers.xlsx
+++ b/settings/tickers.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE802E9-8223-40D7-A352-233CD81C7B48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4800" yWindow="2030" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,103 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>LRCX</t>
+  </si>
+  <si>
+    <t>NFLX</t>
+  </si>
+  <si>
+    <t>QCOM</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>AMGN</t>
+  </si>
+  <si>
+    <t>ISRG</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>TXN</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>AMAT</t>
+  </si>
+  <si>
+    <t>CTSH</t>
+  </si>
+  <si>
+    <t>BIDU</t>
+  </si>
+  <si>
+    <t>GILD</t>
+  </si>
+  <si>
+    <t>ADBE</t>
+  </si>
+  <si>
+    <t>XLNX</t>
+  </si>
+  <si>
+    <t>QQQ</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>CELG</t>
+  </si>
+  <si>
+    <t>VRTX</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>CSCO</t>
+  </si>
+  <si>
+    <t>ADSK</t>
+  </si>
+  <si>
+    <t>CMCSA</t>
+  </si>
+  <si>
+    <t>BIB</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>CDNS</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +426,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major refactor to the project
</commit_message>
<xml_diff>
--- a/settings/tickers.xlsx
+++ b/settings/tickers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE802E9-8223-40D7-A352-233CD81C7B48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5C1FE0-D68A-49BF-9B44-8854E3B003F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2030" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,109 +20,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>AMZN</t>
-  </si>
-  <si>
-    <t>NVDA</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>LRCX</t>
-  </si>
-  <si>
-    <t>NFLX</t>
-  </si>
-  <si>
-    <t>QCOM</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>AMGN</t>
-  </si>
-  <si>
-    <t>ISRG</t>
-  </si>
-  <si>
-    <t>GOOG</t>
-  </si>
-  <si>
-    <t>TXN</t>
-  </si>
-  <si>
-    <t>INTC</t>
-  </si>
-  <si>
-    <t>AMAT</t>
-  </si>
-  <si>
-    <t>CTSH</t>
-  </si>
-  <si>
-    <t>BIDU</t>
-  </si>
-  <si>
-    <t>GILD</t>
-  </si>
-  <si>
-    <t>ADBE</t>
-  </si>
-  <si>
-    <t>XLNX</t>
-  </si>
-  <si>
-    <t>QQQ</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>ATVI</t>
-  </si>
-  <si>
-    <t>CELG</t>
-  </si>
-  <si>
-    <t>VRTX</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>CSCO</t>
-  </si>
-  <si>
-    <t>ADSK</t>
-  </si>
-  <si>
-    <t>CMCSA</t>
-  </si>
-  <si>
-    <t>BIB</t>
-  </si>
-  <si>
-    <t>COST</t>
-  </si>
-  <si>
-    <t>CDNS</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="38">
+  <si>
+    <t>VCIT</t>
+  </si>
+  <si>
+    <t>ITE</t>
+  </si>
+  <si>
+    <t>JNK</t>
+  </si>
+  <si>
+    <t>BNDX</t>
+  </si>
+  <si>
+    <t>PSK</t>
+  </si>
+  <si>
+    <t>DJCI</t>
+  </si>
+  <si>
+    <t>VAW</t>
+  </si>
+  <si>
+    <t>IAU</t>
+  </si>
+  <si>
+    <t>IEO</t>
+  </si>
+  <si>
+    <t>WOOD</t>
+  </si>
+  <si>
+    <t>VIG</t>
+  </si>
+  <si>
+    <t>VIGI</t>
+  </si>
+  <si>
+    <t>DVY</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>VYM</t>
+  </si>
+  <si>
+    <t>SDIV</t>
+  </si>
+  <si>
+    <t>VWO</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>VXUS</t>
+  </si>
+  <si>
+    <t>VTV</t>
+  </si>
+  <si>
+    <t>IMTM</t>
+  </si>
+  <si>
+    <t>MTUM</t>
+  </si>
+  <si>
+    <t>VBR</t>
+  </si>
+  <si>
+    <t>VNQ</t>
+  </si>
+  <si>
+    <t>OHI</t>
+  </si>
+  <si>
+    <t>VNQI</t>
+  </si>
+  <si>
+    <t>VDC</t>
+  </si>
+  <si>
+    <t>VDE</t>
+  </si>
+  <si>
+    <t>VFH</t>
+  </si>
+  <si>
+    <t>VHT</t>
+  </si>
+  <si>
+    <t>IGF</t>
+  </si>
+  <si>
+    <t>VIS</t>
+  </si>
+  <si>
+    <t>VGT</t>
+  </si>
+  <si>
+    <t>XTN</t>
+  </si>
+  <si>
+    <t>VPU</t>
+  </si>
+  <si>
+    <t>QAI</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>OLN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,8 +175,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,165 +458,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>